<commit_message>
Germerged + admin kan klassen zien en het rooster daarvan
</commit_message>
<xml_diff>
--- a/KT2/Weekverslagen/Weekverslag week 3 teun.xlsx
+++ b/KT2/Weekverslagen/Weekverslag week 3 teun.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t xml:space="preserve">Maandag 6 maart: </t>
   </si>
@@ -92,7 +92,31 @@
     <t>Donderdag 16 maart:</t>
   </si>
   <si>
-    <t>Niks gedaan ik was ziek</t>
+    <t>Ik was ziek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maandag 20 maart: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absentie nog beter gemaakt </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dinsdag 21 maart: </t>
+  </si>
+  <si>
+    <t>Ervoor zorgen dat mensen je absentie kunnen afkeueren en goed keuren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Woensdag 22 maart: </t>
+  </si>
+  <si>
+    <t>Ervoor zorgen dat de absentie en het rooster beter worden gemaakt en dat het rooster op de goede dag komt van de week</t>
+  </si>
+  <si>
+    <t>Donderdag 23 maart:</t>
+  </si>
+  <si>
+    <t>Ervoor zorgen dat je de klas kan inzien en en daar weer het rooster van die klas kan zien en de leerlingen van de klas</t>
   </si>
 </sst>
 </file>
@@ -438,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,6 +564,38 @@
         <v>21</v>
       </c>
     </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>